<commit_message>
Progression Hospitality - 3265298940 업데이트
</commit_message>
<xml_diff>
--- a/Data/ferny/Progression Hospitality - 3265298940/3265298940.xlsx
+++ b/Data/ferny/Progression Hospitality - 3265298940/3265298940.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.9.1\Progression Hospitality - 3265298940\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Progression Hospitality - 3265298940\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{465A8DDE-E3A3-468B-BF1A-0392D848B041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164EFD0C-4CE2-4E3B-91C7-FBBCC982119D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240714" sheetId="1" r:id="rId1"/>
@@ -22,19 +22,71 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>bjmi0</author>
     <author>RimWorldKorea</author>
   </authors>
   <commentList>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{89C55705-60F4-4382-9F68-46E1E1A5E671}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02 이전의 원문: 'Begin building mechanisms capable of making money from visitors through sales.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 삭제됨. 삭제 이전 번역문: '소형 화석 전시대'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 삭제됨. 삭제 이전 번역문: '중형 화석 전시대'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 삭제됨. 삭제 이전 번역문: '대형 화석 전시대'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="돋움"/>
             <family val="3"/>
-            <charset val="129"/>
           </rPr>
           <t>적용</t>
         </r>
@@ -42,7 +94,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -52,10 +104,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="돋움"/>
             <family val="3"/>
-            <charset val="129"/>
           </rPr>
           <t>안되면</t>
         </r>
@@ -63,7 +114,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -73,10 +124,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="돋움"/>
             <family val="3"/>
-            <charset val="129"/>
           </rPr>
           <t>순서</t>
         </r>
@@ -84,7 +134,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -94,10 +144,9 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="돋움"/>
             <family val="3"/>
-            <charset val="129"/>
           </rPr>
           <t>조절</t>
         </r>
@@ -105,7 +154,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -115,12 +164,37 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="돋움"/>
             <family val="3"/>
-            <charset val="129"/>
           </rPr>
           <t>필요</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (6개)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{6C7C9BDE-320C-4700-8A02-532B39031D67}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2025-05-02에 새로 추가된 노드들 (6개)</t>
         </r>
       </text>
     </comment>
@@ -129,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="92">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -161,6 +235,9 @@
     <t>Amenities</t>
   </si>
   <si>
+    <t>접대</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Ferny_BasicRetail.label</t>
   </si>
   <si>
@@ -173,13 +250,16 @@
     <t>Basic retail</t>
   </si>
   <si>
+    <t>기본 상업</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Ferny_BasicRetail.description</t>
   </si>
   <si>
     <t>Ferny_BasicRetail.description</t>
   </si>
   <si>
-    <t>Begin building mechanisms capable of making money from visitors through sales.</t>
+    <t>Patches.ThingDef+MedievalVendingMachine.label</t>
   </si>
   <si>
     <t>ResearchTabDef+Ferny_Hospitality.label</t>
@@ -203,6 +283,9 @@
     <t>Museums</t>
   </si>
   <si>
+    <t>박물관</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Ferny_Museums.description</t>
   </si>
   <si>
@@ -212,6 +295,9 @@
     <t>Display your colony's finest history for guests across the Rim to enjoy.</t>
   </si>
   <si>
+    <t>변방계의 손님들이 즐길 수 있도록 식민지의 가장 훌륭한 역사를 전시하세요.</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Ferny_SlotMachines.label</t>
   </si>
   <si>
@@ -224,6 +310,9 @@
     <t>Slot machines</t>
   </si>
   <si>
+    <t>슬롯머신</t>
+  </si>
+  <si>
     <t>ResearchProjectDef+Ferny_SlotMachines.description</t>
   </si>
   <si>
@@ -233,6 +322,9 @@
     <t>Build slot machines for a potentially very profitable casino. Entertain your visitors, and make a little cash on the side.</t>
   </si>
   <si>
+    <t>카지노에 슬롯머신을 건설할 수 있습니다. 방문객은 즐겁게 슬롯머신을 돌리며, 당신은 돈을 법니다.</t>
+  </si>
+  <si>
     <t>ThingDef+Ferny_MerchantBox.label</t>
   </si>
   <si>
@@ -248,6 +340,9 @@
     <t>Merchant box</t>
   </si>
   <si>
+    <t>판매 상자</t>
+  </si>
+  <si>
     <t>ThingDef+Ferny_MerchantBox.description</t>
   </si>
   <si>
@@ -257,6 +352,12 @@
     <t>A merchant box, a low-tech workplace. From here you can manage your restaurant or shop.</t>
   </si>
   <si>
+    <t>웨이터를 위한 작업 공간으로 사용되는 판매 상자입니다. 여기에서 레스토랑을 관리할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>ThingDef+MedievalVendingMachine.label</t>
+  </si>
+  <si>
     <t>MedievalVendingMachine.label</t>
   </si>
   <si>
@@ -266,12 +367,18 @@
     <t>vending shelf</t>
   </si>
   <si>
+    <t>ThingDef+MedievalVendingMachine.description</t>
+  </si>
+  <si>
     <t>MedievalVendingMachine.description</t>
   </si>
   <si>
     <t>A cheap option for vending to guests, an optimal choice for instances where you don't want to setup a full market zone or build vending machines.</t>
   </si>
   <si>
+    <t>ThingDef+BMT_DisplaySmall.label</t>
+  </si>
+  <si>
     <t>BMT_DisplaySmall.label</t>
   </si>
   <si>
@@ -281,79 +388,104 @@
     <t>small fossil display</t>
   </si>
   <si>
+    <t>ThingDef+BMT_DisplayMedium.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+MedievalVendingMachine.description</t>
+  </si>
+  <si>
     <t>BMT_DisplayMedium.label</t>
   </si>
   <si>
     <t>medium fossil display</t>
   </si>
   <si>
+    <t>ThingDef+BMT_DisplayLarge.label</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef</t>
+  </si>
+  <si>
     <t>BMT_DisplayLarge.label</t>
   </si>
   <si>
     <t>large fossil display</t>
   </si>
   <si>
+    <t>ThingDef+CashRegister_CashRegister.description</t>
+  </si>
+  <si>
+    <t>Begin building simple structures capable of making money from visitors.</t>
+  </si>
+  <si>
     <t>CashRegister_CashRegister.description</t>
   </si>
   <si>
     <t>A cash register. From here you can control your restaurant or store.</t>
   </si>
   <si>
-    <t>웨이터를 위한 작업 공간으로 사용되는 판매 상자입니다. 여기에서 레스토랑을 관리할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>슬롯머신</t>
-  </si>
-  <si>
-    <t>변방계의 손님들이 즐길 수 있도록 식민지의 가장 훌륭한 역사를 전시하세요.</t>
-  </si>
-  <si>
-    <t>방문자에게 물건을 팔아 수익을 창출하는 기초적인 상업 구조를 만들어냅니다.</t>
-  </si>
-  <si>
-    <t>접대</t>
-  </si>
-  <si>
-    <t>기본 상업</t>
-  </si>
-  <si>
-    <t>박물관</t>
-  </si>
-  <si>
-    <t>카지노에 슬롯머신을 건설할 수 있습니다. 방문객은 즐겁게 슬롯머신을 돌리며, 당신은 돈을 법니다.</t>
-  </si>
-  <si>
-    <t>판매 상자</t>
-  </si>
-  <si>
-    <t>소형 화석 전시대</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>중형 화석 전시대</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>대형 화석 전시대</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+MedievalVendingMachine.label</t>
-  </si>
-  <si>
-    <t>ThingDef+MedievalVendingMachine.description</t>
-  </si>
-  <si>
-    <t>ThingDef+BMT_DisplaySmall.label</t>
-  </si>
-  <si>
-    <t>ThingDef+BMT_DisplayMedium.label</t>
-  </si>
-  <si>
-    <t>ThingDef+BMT_DisplayLarge.label</t>
-  </si>
-  <si>
-    <t>ThingDef+CashRegister_CashRegister.description</t>
+    <t>Patches.ThingDef+CashRegister_CashRegister.description</t>
+  </si>
+  <si>
+    <t>A cash register. From here you can manage your restaurant or shop.</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+DBHSaunaHeaterElec.label</t>
+  </si>
+  <si>
+    <t>DBHSaunaHeaterElec.label</t>
+  </si>
+  <si>
+    <t>Hospitality: Spa</t>
+  </si>
+  <si>
+    <t>electric sauna heater</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+DBHSaunaHeaterLog.label</t>
+  </si>
+  <si>
+    <t>DBHSaunaHeaterLog.label</t>
+  </si>
+  <si>
+    <t>fueled sauna heater</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+DBHSaunaSeating.label</t>
+  </si>
+  <si>
+    <t>DBHSaunaSeating.label</t>
+  </si>
+  <si>
+    <t>sauna seating</t>
+  </si>
+  <si>
+    <t>자판기 선반</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>방문자에게 물건을 팔아 수익을 창출하는 간단한 구조물을 만들 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>간단하게 손님에게 물건을 팔 수 있습니다. 대규모 판매 구역을 설정하거나 자동 판매기를 만들고 싶지 않은 경우 최적의 선택입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>음식점과 상점을 관리할 수 있는 금전 등록기입니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전기 사우나 난방기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>사우나 좌석</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>화력발전 사우나 난방기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -374,34 +506,33 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="돋움"/>
       <family val="3"/>
-      <charset val="129"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +542,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
       </patternFill>
     </fill>
   </fills>
@@ -438,19 +584,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="메모" xfId="1" builtinId="10"/>
+  <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -751,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -803,299 +948,419 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>56</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="2"/>
+      <c r="B21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>